<commit_message>
adding comments to code
</commit_message>
<xml_diff>
--- a/dados/receitas_drinks.xlsx
+++ b/dados/receitas_drinks.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="109">
   <si>
     <t>drink</t>
   </si>
@@ -323,12 +323,6 @@
     <t>laranja</t>
   </si>
   <si>
-    <t>simple syrup</t>
-  </si>
-  <si>
-    <t>calda de mel</t>
-  </si>
-  <si>
     <t>colher de chá</t>
   </si>
   <si>
@@ -336,9 +330,6 @@
   </si>
   <si>
     <t>chuchadas</t>
-  </si>
-  <si>
-    <t>calda de açúcar</t>
   </si>
   <si>
     <t>uvas brancas</t>
@@ -429,11 +420,11 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -920,7 +911,7 @@
       <c r="B16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -931,16 +922,16 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -951,10 +942,10 @@
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -968,10 +959,10 @@
       <c r="A19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -4599,7 +4590,7 @@
       <c r="D38" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="1" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4718,8 +4709,8 @@
       <c r="D45" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>103</v>
+      <c r="E45" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="46">
@@ -4769,8 +4760,8 @@
       <c r="D48" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>104</v>
+      <c r="E48" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="49">
@@ -4791,50 +4782,50 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C50" s="8">
         <v>1.0</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="11">
-        <v>3.0</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C52" s="8">
         <v>1.0</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -4842,27 +4833,27 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C53" s="8">
         <v>2.0</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C54" s="1">
@@ -4874,7 +4865,7 @@
       <c r="E54" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G54" s="12"/>
+      <c r="G54" s="11"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
@@ -4892,7 +4883,7 @@
       <c r="E55" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G55" s="12"/>
+      <c r="G55" s="11"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
@@ -4910,7 +4901,7 @@
       <c r="E56" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G56" s="12"/>
+      <c r="G56" s="11"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
@@ -4919,16 +4910,16 @@
       <c r="B57" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C57" s="4">
+      <c r="C57" s="1">
         <v>15.0</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G57" s="12"/>
+      <c r="E57" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G57" s="11"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
@@ -4941,9 +4932,9 @@
         <v>5.0</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G58" s="12"/>
+        <v>106</v>
+      </c>
+      <c r="G58" s="11"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
@@ -4952,7 +4943,7 @@
       <c r="B59" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="11">
+      <c r="C59" s="8">
         <v>1.0</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -4969,7 +4960,7 @@
       <c r="B60" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C60" s="11">
+      <c r="C60" s="8">
         <v>2.0</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -4980,17 +4971,17 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C61" s="11">
+      <c r="C61" s="8">
         <v>3.0</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>87</v>
@@ -5003,11 +4994,11 @@
       <c r="B62" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="11">
+      <c r="C62" s="8">
         <v>1.0</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>99</v>
@@ -5020,11 +5011,11 @@
       <c r="B63" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C63" s="11">
+      <c r="C63" s="8">
         <v>2.0</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>95</v>
@@ -5037,7 +5028,7 @@
       <c r="B64" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="11">
+      <c r="C64" s="8">
         <v>2.0</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -5054,7 +5045,7 @@
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C65" s="11">
+      <c r="C65" s="8">
         <v>1.0</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -5071,7 +5062,7 @@
       <c r="B66" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C66" s="11">
+      <c r="C66" s="8">
         <v>1.0</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -5088,7 +5079,7 @@
       <c r="B67" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C67" s="11">
+      <c r="C67" s="8">
         <v>1.0</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -5105,7 +5096,7 @@
       <c r="B68" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C68" s="11">
+      <c r="C68" s="12">
         <v>60.0</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -5122,7 +5113,7 @@
       <c r="B69" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C69" s="11">
+      <c r="C69" s="12">
         <v>30.0</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -5139,7 +5130,7 @@
       <c r="B70" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="11">
+      <c r="C70" s="12">
         <v>7.5</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -5156,11 +5147,11 @@
       <c r="B71" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C71" s="11">
+      <c r="C71" s="12">
         <v>6.0</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>98</v>

</xml_diff>